<commit_message>
albert i jordi vagos
</commit_message>
<xml_diff>
--- a/api/out/XLSX/SGAE_ResumAutoliquidacions.xlsx
+++ b/api/out/XLSX/SGAE_ResumAutoliquidacions.xlsx
@@ -598,91 +598,45 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>Testing_Orchestra</t>
-        </is>
-      </c>
-      <c r="C4" s="14" t="inlineStr">
-        <is>
-          <t>26/11/2023</t>
-        </is>
-      </c>
-      <c r="D4" s="14" t="inlineStr">
-        <is>
-          <t>30/11/2023</t>
-        </is>
-      </c>
-      <c r="E4" s="12" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="F4" s="12" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="G4" s="12" t="inlineStr">
-        <is>
-          <t>Test_name</t>
-        </is>
+          <t>SardanaRip</t>
+        </is>
+      </c>
+      <c r="C4" s="14" t="n">
+        <v/>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v/>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v/>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v/>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v/>
       </c>
       <c r="H4" s="12" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>Olaaa</t>
         </is>
       </c>
       <c r="I4" s="12" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>Olaaa</t>
         </is>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" s="8">
-      <c r="A5" s="12" t="inlineStr">
-        <is>
-          <t>---</t>
-        </is>
-      </c>
-      <c r="B5" s="13" t="inlineStr">
-        <is>
-          <t>Testing_Orchestra</t>
-        </is>
-      </c>
-      <c r="C5" s="14" t="inlineStr">
-        <is>
-          <t>26/11/2023</t>
-        </is>
-      </c>
-      <c r="D5" s="14" t="inlineStr">
-        <is>
-          <t>30/11/2023</t>
-        </is>
-      </c>
-      <c r="E5" s="12" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="F5" s="12" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="G5" s="12" t="inlineStr">
-        <is>
-          <t>Test_name</t>
-        </is>
-      </c>
-      <c r="H5" s="12" t="inlineStr">
-        <is>
-          <t>Testing2</t>
-        </is>
-      </c>
-      <c r="I5" s="12" t="inlineStr">
-        <is>
-          <t>Testing2</t>
-        </is>
-      </c>
+      <c r="A5" s="12" t="n"/>
+      <c r="B5" s="13" t="n"/>
+      <c r="C5" s="14" t="n"/>
+      <c r="D5" s="14" t="n"/>
+      <c r="E5" s="12" t="n"/>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="12" t="n"/>
+      <c r="H5" s="12" t="n"/>
+      <c r="I5" s="12" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1" s="8">
       <c r="A6" s="12" t="n"/>

</xml_diff>